<commit_message>
Add more responses to survey
</commit_message>
<xml_diff>
--- a/all/Age.xlsx
+++ b/all/Age.xlsx
@@ -477,10 +477,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3" t="n">
         <v>6</v>

</xml_diff>